<commit_message>
updates to anadromous functions
</commit_message>
<xml_diff>
--- a/data/stressor_response_demo.xlsx
+++ b/data/stressor_response_demo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C331B-DBBB-421F-BBF8-4FA3B6312076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB68D38-BD76-41E3-AEE4-92D77AA91D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
@@ -367,11 +367,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14225,7 +14224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -14456,7 +14455,7 @@
         <v>33</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="7" t="s">
         <v>52</v>
       </c>
@@ -14485,7 +14484,7 @@
         <v>33</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="7" t="s">
         <v>52</v>
       </c>
@@ -14514,7 +14513,7 @@
         <v>33</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="7" t="s">
         <v>52</v>
       </c>
@@ -14543,7 +14542,7 @@
         <v>33</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="9"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="7" t="s">
         <v>52</v>
       </c>
@@ -14572,7 +14571,7 @@
         <v>33</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="9"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="7" t="s">
         <v>52</v>
       </c>
@@ -14601,7 +14600,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="9"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="7" t="s">
         <v>52</v>
       </c>
@@ -14630,7 +14629,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="7" t="s">
         <v>52</v>
       </c>
@@ -14659,7 +14658,7 @@
         <v>33</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="9"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="7" t="s">
         <v>52</v>
       </c>
@@ -14688,7 +14687,7 @@
         <v>33</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="9"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="7" t="s">
         <v>52</v>
       </c>
@@ -14719,7 +14718,7 @@
       <c r="H16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="7" t="s">
         <v>51</v>
       </c>
@@ -14750,7 +14749,7 @@
       <c r="H17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="8"/>
       <c r="J17" s="7" t="s">
         <v>51</v>
       </c>
@@ -14781,15 +14780,15 @@
       <c r="H18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="8"/>
       <c r="J18" s="7" t="s">
         <v>51</v>
       </c>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -16793,8 +16792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>